<commit_message>
Add Login feature file - Gherkin Test
</commit_message>
<xml_diff>
--- a/Data Files/login-invalidemail.xlsx
+++ b/Data Files/login-invalidemail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silmi\Katalon Studio\Magento - Web Automation Testing\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8DAEE2-0155-40B4-97EF-BC03357AEC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3EC14F-19E6-4015-AB03-29D9C30C792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02267841-48DA-40D1-97EE-DC2B2DFE1206}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>invalid email</t>
+  </si>
+  <si>
+    <t>mail.unregistered@test.com</t>
+  </si>
+  <si>
+    <t>ABCde!12350</t>
+  </si>
+  <si>
+    <t>incorrect account</t>
   </si>
 </sst>
 </file>
@@ -430,17 +439,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6616D-1622-4008-B79F-7A192A0AE8D0}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -498,10 +507,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{66D0D9C7-B501-474A-9EA5-7079073F0CF7}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{BDBE8A2A-6210-4A6B-9974-B49209C0A8C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>